<commit_message>
AA16 and observed variables
AA16 and observed variables
</commit_message>
<xml_diff>
--- a/data/observed_variable_description.xlsx
+++ b/data/observed_variable_description.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THUY TRANG\Documents\GitHub\MMB_forecast_application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F3EB24-163D-4DB4-AFD5-9B9192BBE66B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -127,12 +126,45 @@
   </si>
   <si>
     <t>cp_q_obs</t>
+  </si>
+  <si>
+    <t>gdp_q_AA16_obs</t>
+  </si>
+  <si>
+    <t>Real GDP minus NETEXPORT, net growth, aggregate</t>
+  </si>
+  <si>
+    <t>ΔLN(GDPCTPI-(NETEXP/GDPTCPI))*100</t>
+  </si>
+  <si>
+    <t>i_q_AA16_obs</t>
+  </si>
+  <si>
+    <t>Norminal investment, net growth, aggrrgate</t>
+  </si>
+  <si>
+    <t>Nominal investment growth</t>
+  </si>
+  <si>
+    <t>c_q_AA16_obs</t>
+  </si>
+  <si>
+    <t>Consumption growth</t>
+  </si>
+  <si>
+    <t>ΔLN(PCESVC96+PCNDGC96)*100</t>
+  </si>
+  <si>
+    <t>ΔLN(FPI+PCDGCC96)*100</t>
+  </si>
+  <si>
+    <t>Consumption, net growth, aggregate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -443,11 +475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,6 +602,48 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Vintage generation code update
</commit_message>
<xml_diff>
--- a/data/observed_variable_description.xlsx
+++ b/data/observed_variable_description.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Documents\GitHub\MMB_forecast_application\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6B8BF7-3C09-4828-8410-AB39833DEE11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818EF7BF-6686-4485-9070-FBC918725804}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="23880" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
   <si>
     <t>id</t>
   </si>
@@ -33,9 +33,6 @@
     <t>construction</t>
   </si>
   <si>
-    <t>Real GDP, net growth, aggregate</t>
-  </si>
-  <si>
     <t>ΔLN(GDPC1)*100</t>
   </si>
   <si>
@@ -51,15 +48,9 @@
     <t>ΔLN(GDPCTPI)*100</t>
   </si>
   <si>
-    <t>Real investment, net growth, aggregate, deflated by GDP deflator</t>
-  </si>
-  <si>
     <t>ΔLN(FPI/GDPCTPI)*100</t>
   </si>
   <si>
-    <t>Real consumption, net growth, aggregate, deflated by GDP deflator</t>
-  </si>
-  <si>
     <t>ΔLN(PCE/GDPCTPI)*100</t>
   </si>
   <si>
@@ -78,30 +69,15 @@
     <t>Real GDP growth</t>
   </si>
   <si>
-    <t>GDP deflator</t>
-  </si>
-  <si>
     <t>Fedeal funds rate</t>
   </si>
   <si>
-    <t>Real investment growth</t>
-  </si>
-  <si>
-    <t>Real consumption growth</t>
-  </si>
-  <si>
-    <t>Credit spreads</t>
-  </si>
-  <si>
     <t>Real wage growth</t>
   </si>
   <si>
     <t>Effective federal funds rate, quarterly average</t>
   </si>
   <si>
-    <t>spread between BAA corporate bond yield and 10 yr Treasury bond yield, quarterly average</t>
-  </si>
-  <si>
     <t>gdp_q_AA16_obs</t>
   </si>
   <si>
@@ -127,15 +103,6 @@
   </si>
   <si>
     <t>ffr_obs</t>
-  </si>
-  <si>
-    <t>fpi_rgd_obs</t>
-  </si>
-  <si>
-    <t>pce_rgd_obs</t>
-  </si>
-  <si>
-    <t>sp_baa10y_obs</t>
   </si>
   <si>
     <t>wage_rgd_obs</t>
@@ -267,6 +234,120 @@
   </si>
   <si>
     <t>ΔLN(CES2000000008)</t>
+  </si>
+  <si>
+    <t>Real GDP, net growth,  deflated by GDP deflator</t>
+  </si>
+  <si>
+    <t>GDP deflator growth</t>
+  </si>
+  <si>
+    <t>ifi_rgd_obs</t>
+  </si>
+  <si>
+    <t>Real fixed invest., net growth, deflated by GDP deflator</t>
+  </si>
+  <si>
+    <t>Real invest. growth: fixed invest.</t>
+  </si>
+  <si>
+    <t>c_rgd_obs</t>
+  </si>
+  <si>
+    <t>Real cons., net growth, deflated by GDP deflator</t>
+  </si>
+  <si>
+    <t>Real cons. growth</t>
+  </si>
+  <si>
+    <t>networth_rgd_obs</t>
+  </si>
+  <si>
+    <t>Real DJ Wilshere 5000 TM index, net growth, deflated by GDP deflator</t>
+  </si>
+  <si>
+    <t>Real net worth growth</t>
+  </si>
+  <si>
+    <t>ΔLN(WILL5000IND/GDPCTPI)*100</t>
+  </si>
+  <si>
+    <t>credit_rgd_obs</t>
+  </si>
+  <si>
+    <t>Real liabilities of nonfinancial business, net growth, deflated by GDP deflator</t>
+  </si>
+  <si>
+    <t>Real credit growth</t>
+  </si>
+  <si>
+    <t>ΔLN(BOGZ1FL144104005Q/GDPCTPI)*100</t>
+  </si>
+  <si>
+    <t>cnds_rim_obs</t>
+  </si>
+  <si>
+    <t>Real non-durable goods and sevices cons., net growth, deflated by implicit deflator</t>
+  </si>
+  <si>
+    <t>Real cons. growth: nondurable goods and services</t>
+  </si>
+  <si>
+    <t>ΔLN(PCESC96+PCENDC96)*100</t>
+  </si>
+  <si>
+    <t>igid_rim_obs</t>
+  </si>
+  <si>
+    <t>Real gross invest. and durable goods cons., net growth, deflated by implicit deflator</t>
+  </si>
+  <si>
+    <t>Real invest. growth: durable goods and gross invest.</t>
+  </si>
+  <si>
+    <t>ΔLN(PCEDGC96+GPDIC1)*100</t>
+  </si>
+  <si>
+    <t>igiddef_rgd_obs</t>
+  </si>
+  <si>
+    <t>Real gross invest. and durable goods cons. deflator, net growth, deflated by GDP deflator</t>
+  </si>
+  <si>
+    <t>Real invest. (durable goods and gross invest.) deflator growth</t>
+  </si>
+  <si>
+    <t>ΔLN(((GPDI+PCEDG)/(GPDIC1+PCEDGC96))/GDPCTPI)*100</t>
+  </si>
+  <si>
+    <t>hours_cmr14_obs</t>
+  </si>
+  <si>
+    <t>Hours in the CMR14 model</t>
+  </si>
+  <si>
+    <t>LN(HOANBS/CNP16OV)</t>
+  </si>
+  <si>
+    <t>baag10_obs</t>
+  </si>
+  <si>
+    <t>difference between BAA corporate bond yield and 10yr Treasury bond yield, quarterly average</t>
+  </si>
+  <si>
+    <t>Credit spread</t>
+  </si>
+  <si>
+    <t>g10ffr_obs</t>
+  </si>
+  <si>
+    <t>difference between 10yr Treasury bond yield and effective federal funds rate, quarterly average</t>
+  </si>
+  <si>
+    <t>Term premium</t>
+  </si>
+  <si>
+    <t>(DGS10-DFF)/4</t>
   </si>
 </sst>
 </file>
@@ -602,18 +683,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:D25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" customWidth="1"/>
-    <col min="2" max="2" width="84" customWidth="1"/>
-    <col min="3" max="3" width="37.453125" customWidth="1"/>
-    <col min="4" max="4" width="40.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="86.140625" customWidth="1"/>
+    <col min="3" max="3" width="57.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -621,10 +702,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -632,282 +713,380 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75">
+      <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="15.75">
+      <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.5">
-      <c r="A18" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.5">
-      <c r="A19" s="1" t="s">
+    <row r="29" spans="1:4" ht="15.75">
+      <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.5">
-      <c r="A20" s="1" t="s">
+    <row r="30" spans="1:4" ht="15.75">
+      <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="2" t="s">
+    </row>
+    <row r="31" spans="1:4" ht="15.75">
+      <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.5">
-      <c r="A21" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="2" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="15.75">
+      <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.5">
-      <c r="A22" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.5">
-      <c r="A23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.5">
-      <c r="A24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.5">
-      <c r="A25" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update in obs var
</commit_message>
<xml_diff>
--- a/data/observed_variable_description.xlsx
+++ b/data/observed_variable_description.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="210">
   <si>
     <t>id</t>
   </si>
@@ -651,6 +651,18 @@
   </si>
   <si>
     <t>LN(FGS)</t>
+  </si>
+  <si>
+    <t>cnds_nom_demean_obs</t>
+  </si>
+  <si>
+    <t>Nominal cons. on non-durables and services, net growth, demean</t>
+  </si>
+  <si>
+    <t>Nominal consumption growth</t>
+  </si>
+  <si>
+    <t>demean:ΔLN(PCEND+PCES)*100</t>
   </si>
 </sst>
 </file>
@@ -730,7 +742,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -748,6 +760,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1029,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1588,7 +1601,7 @@
       <c r="A36" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1602,7 +1615,7 @@
       <c r="A37" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="9" t="s">
         <v>191</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1616,7 +1629,7 @@
       <c r="A38" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="9" t="s">
         <v>194</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1630,7 +1643,7 @@
       <c r="A39" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="9" t="s">
         <v>198</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1654,143 +1667,160 @@
         <v>203</v>
       </c>
     </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="B42" s="9"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>189</v>
+        <v>46</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>53</v>
+        <v>189</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/zexisun/MMB_forecast_application"
This reverts commit 91d94af7ff53adb35aeac65fddc7d7a239e15aa6, reversing
changes made to c4be6e1284bde445eb1c38c458fa4fafb4636e60.
</commit_message>
<xml_diff>
--- a/data/observed_variable_description.xlsx
+++ b/data/observed_variable_description.xlsx
@@ -5,27 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Documents\GitHub\MMB_forecast_application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1C0614-4064-47CF-AEC0-F3CEFEB3436C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55128C28-996A-417D-B8B0-07F44871E20F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="23205" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="530" windowWidth="17430" windowHeight="10270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="199">
   <si>
     <t>id</t>
   </si>
@@ -78,12 +84,24 @@
     <t>Effective federal funds rate, quarterly average</t>
   </si>
   <si>
+    <t>gdp_q_AA16_obs</t>
+  </si>
+  <si>
     <t>Real GDP minus NETEXPORT, net growth, aggregate</t>
   </si>
   <si>
+    <t>i_q_AA16_obs</t>
+  </si>
+  <si>
+    <t>Norminal investment, net growth, aggrrgate</t>
+  </si>
+  <si>
     <t>Nominal investment growth</t>
   </si>
   <si>
+    <t>c_q_AA16_obs</t>
+  </si>
+  <si>
     <t>gdp_rgd_obs</t>
   </si>
   <si>
@@ -94,6 +112,21 @@
   </si>
   <si>
     <t>wage_rgd_obs</t>
+  </si>
+  <si>
+    <t>ΔLN(GPDI+PCDG)*100</t>
+  </si>
+  <si>
+    <t>Norminal consumption, net growth, aggregate</t>
+  </si>
+  <si>
+    <t>ΔLN(PCES+PCND)*100</t>
+  </si>
+  <si>
+    <t>Nominal consumption growth</t>
+  </si>
+  <si>
+    <t>ΔLN((GDPC1-NETEXC)/CLF16OV)*100</t>
   </si>
   <si>
     <t>Real consumption</t>
@@ -344,6 +377,9 @@
     <t>gdpl_rgd_obs</t>
   </si>
   <si>
+    <t>cpi_obs</t>
+  </si>
+  <si>
     <t>Bank lending tightening index</t>
   </si>
   <si>
@@ -595,69 +631,6 @@
   </si>
   <si>
     <t>i_nom_obs</t>
-  </si>
-  <si>
-    <t>gdpnoexp_obs</t>
-  </si>
-  <si>
-    <t>Norminal investment, net growth, aggregate, investment and durable good</t>
-  </si>
-  <si>
-    <t>i_A16_obs</t>
-  </si>
-  <si>
-    <t>hours_A16_obs</t>
-  </si>
-  <si>
-    <t>Hours in A16 model</t>
-  </si>
-  <si>
-    <t>demean: ΔLN((GDP-NETEXP)/GDPCTPI)*100</t>
-  </si>
-  <si>
-    <t>demean: ΔLN(GPDI+PCDG)*100</t>
-  </si>
-  <si>
-    <t>fgs_obs</t>
-  </si>
-  <si>
-    <t>Financial gap share, net grwoth, aggregate</t>
-  </si>
-  <si>
-    <t>Nominal hour growth</t>
-  </si>
-  <si>
-    <t>Nominal financial gap growth</t>
-  </si>
-  <si>
-    <t>wage_rgd_demean_obs</t>
-  </si>
-  <si>
-    <t>Real wage growth, net growth, deflated by GDP deflator, demean</t>
-  </si>
-  <si>
-    <t>demean:ΔLN(COMPNFB/GDPCTPI)*100</t>
-  </si>
-  <si>
-    <t>(demean: LN(TOTLQ*100/CLF16OV))*100</t>
-  </si>
-  <si>
-    <t>LN(FGS)</t>
-  </si>
-  <si>
-    <t>cnds_nom_demean_obs</t>
-  </si>
-  <si>
-    <t>Nominal cons. on non-durables and services, net growth, demean</t>
-  </si>
-  <si>
-    <t>Nominal consumption growth</t>
-  </si>
-  <si>
-    <t>demean:ΔLN(PCEND+PCES)*100</t>
-  </si>
-  <si>
-    <t>cpil_obs</t>
   </si>
 </sst>
 </file>
@@ -687,7 +660,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -706,28 +679,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -737,7 +695,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -754,12 +712,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{4319CBA9-AE78-42AF-8F0F-23C812B78263}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1037,19 +993,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="86.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.54296875" style="1" customWidth="1"/>
     <col min="4" max="4" width="54" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1066,15 +1022,15 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -1083,29 +1039,29 @@
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>16</v>
@@ -1117,46 +1073,46 @@
         <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
@@ -1168,655 +1124,610 @@
         <v>3</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
-        <v>209</v>
+        <v>114</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29">
       <c r="A22" s="5" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="29">
       <c r="A23" s="5" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="5" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="5" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B36" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>194</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>190</v>
+        <v>19</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>195</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>193</v>
+        <v>22</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>198</v>
+        <v>30</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>204</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>202</v>
+        <v>34</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>206</v>
+        <v>37</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>207</v>
+        <v>39</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>208</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="B42" s="9"/>
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="1" t="s">
-        <v>25</v>
+      <c r="A43" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>31</v>
+      <c r="A44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>38</v>
+        <v>198</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>44</v>
+        <v>60</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data. Python files and Matlab files updates
</commit_message>
<xml_diff>
--- a/data/observed_variable_description.xlsx
+++ b/data/observed_variable_description.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Documents\GitHub\MMB_forecast_application\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C30A7D0-AA94-4463-A76D-96C0E0EC367D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F2BE9F-DAC3-4C33-B812-3A79F4FF29D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="530" windowWidth="15920" windowHeight="10270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="990" windowWidth="27900" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1186,19 +1186,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="86.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="104" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1558,24 +1558,24 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="29">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="29">
+    <row r="23" spans="1:5" ht="30">
       <c r="A23" s="4" t="s">
         <v>151</v>
       </c>
@@ -1627,19 +1627,19 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1660,488 +1660,495 @@
         <v>249</v>
       </c>
     </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="A29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="A30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="A31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B32" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C32" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D32" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B33" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C33" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D33" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C34" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D34" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E34" s="4"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>17</v>
+        <v>177</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>18</v>
+        <v>185</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>15</v>
+        <v>192</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D42" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="B43" s="9"/>
-    </row>
-    <row r="44" spans="1:4">
+    <row r="42" spans="1:5">
+      <c r="B42" s="9"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="45" spans="1:5">
+      <c r="A45" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="2" t="s">
-        <v>43</v>
+      <c r="A52" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" s="3" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="10" customFormat="1">
-      <c r="A55" s="10" t="s">
+    <row r="54" spans="1:4" s="10" customFormat="1">
+      <c r="A54" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B54" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C54" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D54" s="10" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="2" t="s">
+    <row r="55" spans="1:4">
+      <c r="A55" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B55" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C55" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="D55" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="12" customFormat="1">
-      <c r="A57" s="12" t="s">
+    <row r="56" spans="1:4" s="12" customFormat="1">
+      <c r="A56" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C56" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D56" s="12" t="s">
         <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="10" customFormat="1">
+      <c r="A57" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="10" customFormat="1">
       <c r="A58" s="10" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="10" customFormat="1">
-      <c r="A59" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B59" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C58" s="11" t="s">
         <v>214</v>
       </c>
+      <c r="D58" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="D59" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>23</v>
+        <v>222</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>213</v>
+      <c r="A61" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>228</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="10" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>228</v>
+        <v>217</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="10" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="C64" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D64" s="11" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65" spans="3:3">
       <c r="C65" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" s="1" t="s">
-        <v>233</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="3:3">
       <c r="C67" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3">
-      <c r="C68" s="1" t="s">
         <v>234</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implement CMR14 and KR15_FF, include CBHPI, code revision
</commit_message>
<xml_diff>
--- a/data/observed_variable_description.xlsx
+++ b/data/observed_variable_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107B8FFB-7A27-43E4-B392-013508A38CB8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCFDAA8-7918-4FCD-9A74-346ABB3734D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="990" windowWidth="27900" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="258">
   <si>
     <t>id</t>
   </si>
@@ -513,18 +513,9 @@
     <t>dlnDin</t>
   </si>
   <si>
-    <t>houseprice_obs</t>
-  </si>
-  <si>
-    <t>House price index, net growth</t>
-  </si>
-  <si>
     <t>House price growth</t>
   </si>
   <si>
-    <t>ΔLN(HPINDEX)*100</t>
-  </si>
-  <si>
     <t>credit_nom_obs</t>
   </si>
   <si>
@@ -790,6 +781,33 @@
   </si>
   <si>
     <t>Divide by mean: AWHNONAG*CE16OV/CNP16OV</t>
+  </si>
+  <si>
+    <t>networth_rgd_cmr14_obs</t>
+  </si>
+  <si>
+    <t>Hours in the SW07 model, demeaned</t>
+  </si>
+  <si>
+    <t>Hours in the FRBEDO08 model, divided by mean</t>
+  </si>
+  <si>
+    <t>Real DJ Wilshere 5000 TM index in the CMR14 model, gross growth, deflated by GDP deflator, demeaned</t>
+  </si>
+  <si>
+    <t>Real net worth growth in the CMR14 model</t>
+  </si>
+  <si>
+    <t>Subtract by mean and then take exponential: ΔLN(WILL5000IND/GDPCTPI)</t>
+  </si>
+  <si>
+    <t>ΔLN(CBHPI)*100</t>
+  </si>
+  <si>
+    <t>hp_nom_obs</t>
+  </si>
+  <si>
+    <t>Nominal house price index, net growth</t>
   </si>
 </sst>
 </file>
@@ -819,7 +837,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -829,12 +847,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,7 +887,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -885,20 +897,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1186,15 +1194,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29" style="1" customWidth="1"/>
     <col min="2" max="2" width="86.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="57.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="104" style="1" customWidth="1"/>
@@ -1334,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1359,13 +1367,13 @@
         <v>90</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>89</v>
+        <v>250</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>89</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>139</v>
@@ -1424,7 +1432,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>102</v>
@@ -1469,7 +1477,7 @@
       <c r="D16" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1484,7 +1492,7 @@
         <v>119</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>120</v>
@@ -1501,7 +1509,7 @@
         <v>124</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>121</v>
@@ -1535,7 +1543,7 @@
         <v>136</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>133</v>
@@ -1546,13 +1554,13 @@
         <v>137</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>138</v>
+        <v>251</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>139</v>
@@ -1562,7 +1570,7 @@
       <c r="A22" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="11" t="s">
         <v>148</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1579,48 +1587,48 @@
       <c r="A23" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>152</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>153</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="E24" s="5" t="s">
+      <c r="D24" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>157</v>
@@ -1628,16 +1636,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B26" s="13" t="s">
         <v>167</v>
       </c>
+      <c r="B26" s="11" t="s">
+        <v>164</v>
+      </c>
       <c r="C26" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>158</v>
@@ -1645,19 +1653,19 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>249</v>
-      </c>
       <c r="E27" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1765,391 +1773,406 @@
       </c>
       <c r="E34" s="4"/>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>180</v>
-      </c>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E35" s="4"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>183</v>
+        <v>175</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B40" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="B42" s="9"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>234</v>
-      </c>
+      <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>235</v>
+      <c r="D45" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>174</v>
+        <v>40</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B52" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="14" t="s">
+      <c r="D52" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" s="10" customFormat="1">
-      <c r="A54" s="10" t="s">
+      <c r="D53" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="8" customFormat="1">
+      <c r="A55" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B56" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="C54" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D54" s="10" t="s">
+      <c r="D56" s="9" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="12" customFormat="1">
-      <c r="A56" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="10" customFormat="1">
       <c r="A57" s="10" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>225</v>
+        <v>14</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="10" customFormat="1">
-      <c r="A58" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="8" customFormat="1">
+      <c r="A58" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="8" customFormat="1">
+      <c r="A59" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="B58" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>206</v>
+      <c r="C59" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D60" s="11" t="s">
+      <c r="B64" s="8" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
       <c r="C64" s="1" t="s">
-        <v>231</v>
+        <v>207</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="65" spans="3:3">
       <c r="C65" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" s="1" t="s">
-        <v>82</v>
+        <v>229</v>
       </c>
     </row>
     <row r="67" spans="3:3">
       <c r="C67" s="1" t="s">
-        <v>233</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data trial update kailong
</commit_message>
<xml_diff>
--- a/data/observed_variable_description.xlsx
+++ b/data/observed_variable_description.xlsx
@@ -5,20 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KaiLong\Documents\GitHub\MMB_forecast_application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9674D89-BA66-472D-8EA3-FDF7D6DF5062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3A7158-0467-4061-9F5C-13479BB4B2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="9720" yWindow="120" windowWidth="16035" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1205,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
new observed variables and updated mod file of HL16
</commit_message>
<xml_diff>
--- a/data/observed_variable_description.xlsx
+++ b/data/observed_variable_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiran/Documents/GitHub/MMB_forecast_application/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E27E769-0C5E-42EC-BA6A-BE4E3670E392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A5870-33FD-994B-A7F2-1D0B43B99971}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="21720" yWindow="2440" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="283">
   <si>
     <t>id</t>
   </si>
@@ -822,13 +822,73 @@
   </si>
   <si>
     <t>ΔLN(CE16OV)*100</t>
+  </si>
+  <si>
+    <t>pi_obs</t>
+  </si>
+  <si>
+    <t>ΔLN(GDPDEF)</t>
+  </si>
+  <si>
+    <t>q_psi_obs</t>
+  </si>
+  <si>
+    <t>SP500</t>
+  </si>
+  <si>
+    <t>ΔLN(SP500/GDPDEF)</t>
+  </si>
+  <si>
+    <t>l_h_obs</t>
+  </si>
+  <si>
+    <t>Loans to households</t>
+  </si>
+  <si>
+    <t>MORTG/100</t>
+  </si>
+  <si>
+    <t>l_e_obs</t>
+  </si>
+  <si>
+    <t>Loans to entrepreneurs</t>
+  </si>
+  <si>
+    <t>ΔLN(TLBSNNCB/GDPDEF)</t>
+  </si>
+  <si>
+    <t>d_obs</t>
+  </si>
+  <si>
+    <t>Deposits</t>
+  </si>
+  <si>
+    <t>ΔLN(DABSHNO/GDPDEF)</t>
+  </si>
+  <si>
+    <t>i_h_obs</t>
+  </si>
+  <si>
+    <t>Loan rate to households</t>
+  </si>
+  <si>
+    <t>ΔLN(TLBSHNO/GDPDEF)</t>
+  </si>
+  <si>
+    <t>i_e_obs</t>
+  </si>
+  <si>
+    <t>Loan rate to entrepreneurs</t>
+  </si>
+  <si>
+    <t>BAA/100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,7 +968,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -934,10 +994,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1209,21 +1270,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
-    <col min="2" max="2" width="86.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="104" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1303,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1257,7 +1320,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1274,7 +1337,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1291,7 +1354,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>51</v>
       </c>
@@ -1308,7 +1371,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -1325,7 +1388,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -1342,7 +1405,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>80</v>
       </c>
@@ -1359,7 +1422,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>87</v>
       </c>
@@ -1376,7 +1439,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>90</v>
       </c>
@@ -1393,7 +1456,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>92</v>
       </c>
@@ -1410,7 +1473,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>93</v>
       </c>
@@ -1427,7 +1490,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>94</v>
       </c>
@@ -1444,7 +1507,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>191</v>
       </c>
@@ -1461,7 +1524,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>108</v>
       </c>
@@ -1478,7 +1541,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>115</v>
       </c>
@@ -1495,7 +1558,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>116</v>
       </c>
@@ -1512,7 +1575,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>117</v>
       </c>
@@ -1529,7 +1592,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>106</v>
       </c>
@@ -1546,7 +1609,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>107</v>
       </c>
@@ -1563,7 +1626,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>137</v>
       </c>
@@ -1580,7 +1643,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30">
+    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>147</v>
       </c>
@@ -1597,7 +1660,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30">
+    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>151</v>
       </c>
@@ -1614,7 +1677,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>252</v>
       </c>
@@ -1631,7 +1694,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>160</v>
       </c>
@@ -1648,7 +1711,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>167</v>
       </c>
@@ -1665,7 +1728,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>239</v>
       </c>
@@ -1682,7 +1745,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>83</v>
       </c>
@@ -1697,7 +1760,7 @@
       </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>61</v>
       </c>
@@ -1712,7 +1775,7 @@
       </c>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>77</v>
       </c>
@@ -1727,7 +1790,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
@@ -1742,7 +1805,7 @@
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>65</v>
       </c>
@@ -1757,7 +1820,7 @@
       </c>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>69</v>
       </c>
@@ -1772,7 +1835,7 @@
       </c>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>73</v>
       </c>
@@ -1787,7 +1850,7 @@
       </c>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>245</v>
       </c>
@@ -1802,7 +1865,7 @@
       </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>254</v>
       </c>
@@ -1816,7 +1879,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>172</v>
       </c>
@@ -1830,7 +1893,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>174</v>
       </c>
@@ -1844,7 +1907,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>175</v>
       </c>
@@ -1858,7 +1921,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>179</v>
       </c>
@@ -1872,7 +1935,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>183</v>
       </c>
@@ -1886,7 +1949,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>187</v>
       </c>
@@ -1900,10 +1963,10 @@
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="7"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -1917,7 +1980,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -1931,7 +1994,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>30</v>
       </c>
@@ -1945,7 +2008,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>32</v>
       </c>
@@ -1959,7 +2022,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>34</v>
       </c>
@@ -1973,7 +2036,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>37</v>
       </c>
@@ -1987,7 +2050,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>40</v>
       </c>
@@ -2001,7 +2064,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>171</v>
       </c>
@@ -2015,7 +2078,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>43</v>
       </c>
@@ -2029,7 +2092,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>46</v>
       </c>
@@ -2043,7 +2106,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="8" customFormat="1">
+    <row r="56" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>195</v>
       </c>
@@ -2057,7 +2120,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>198</v>
       </c>
@@ -2071,7 +2134,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="10" customFormat="1">
+    <row r="58" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
         <v>226</v>
       </c>
@@ -2085,7 +2148,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="8" customFormat="1">
+    <row r="59" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>220</v>
       </c>
@@ -2099,7 +2162,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="8" customFormat="1">
+    <row r="60" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
         <v>210</v>
       </c>
@@ -2113,7 +2176,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>214</v>
       </c>
@@ -2127,7 +2190,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>215</v>
       </c>
@@ -2141,7 +2204,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>224</v>
       </c>
@@ -2155,7 +2218,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>211</v>
       </c>
@@ -2169,7 +2232,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>218</v>
       </c>
@@ -2183,7 +2246,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>260</v>
       </c>
@@ -2195,6 +2258,83 @@
       </c>
       <c r="D67" s="3" t="s">
         <v>262</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementation of KK14 (not done)
</commit_message>
<xml_diff>
--- a/data/observed_variable_description.xlsx
+++ b/data/observed_variable_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yiran/Documents/GitHub/MMB_forecast_application/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Documents\GitHub\MMB_forecast_application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6A5870-33FD-994B-A7F2-1D0B43B99971}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502C7B34-DFAD-40A7-B3D1-6074F99F93D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21720" yWindow="2440" windowWidth="29040" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="300">
   <si>
     <t>id</t>
   </si>
@@ -882,13 +882,64 @@
   </si>
   <si>
     <t>BAA/100</t>
+  </si>
+  <si>
+    <t>log real private consumption per capita</t>
+  </si>
+  <si>
+    <t>diff(log((PCND+ PCESV)/(index(GDPCTPI*CNP16OV))))-mean(log((PCND+ PCESV)/(index(GDPCTPI*CNP16OV))))</t>
+  </si>
+  <si>
+    <t>hrw_pc_obs</t>
+  </si>
+  <si>
+    <t>log total hours worked per capita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log((PRS85006023* CE16OV)/(index(CNP16OV)))-mean(log((PRS85006023* CE16OV)/(index(CNP16OV))))     </t>
+  </si>
+  <si>
+    <t>log real private investment per capita</t>
+  </si>
+  <si>
+    <t>change of log real private consumption per capita</t>
+  </si>
+  <si>
+    <t>change of log real private investment per capita</t>
+  </si>
+  <si>
+    <t>c_rgpc_obs</t>
+  </si>
+  <si>
+    <t>I_rgpc_obs</t>
+  </si>
+  <si>
+    <t>diff(log((GPDI+ PCDG)/(GDPCTPI*CNP16OV)))-mean(diff(log((GPDI+ PCDG)/(GDPCTPI*CNP16OV))))</t>
+  </si>
+  <si>
+    <t>change of log real government expenditure per capita</t>
+  </si>
+  <si>
+    <t>gexp_rgpc_obs</t>
+  </si>
+  <si>
+    <t>X= (A957RC1Q027SBEA+A787RC1Q027SBEA+AD08RC1Q027SBEA-A918RC1Q027SBEA)/(GDPCTPI*CNP16OV)  ,   diff(X)-mean(diff(X))</t>
+  </si>
+  <si>
+    <t>tau_w_obs</t>
+  </si>
+  <si>
+    <t>log labour tax rate</t>
+  </si>
+  <si>
+    <t>RENTIN-CPROFIT-W255RC1Q027SBEA-PROPINC-A074RC1Q027SBEA-W071RC1Q027SBEA-WASCUR-PROPINC-COE-W780RC1Q027SBEA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1271,22 +1322,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29" style="1" customWidth="1"/>
-    <col min="2" max="2" width="86.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="104" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1354,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -1320,7 +1371,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1337,7 +1388,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1354,7 +1405,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>51</v>
       </c>
@@ -1371,7 +1422,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -1388,7 +1439,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -1405,7 +1456,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>80</v>
       </c>
@@ -1422,7 +1473,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>87</v>
       </c>
@@ -1439,7 +1490,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>90</v>
       </c>
@@ -1456,7 +1507,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>92</v>
       </c>
@@ -1473,7 +1524,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>93</v>
       </c>
@@ -1490,7 +1541,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
         <v>94</v>
       </c>
@@ -1507,7 +1558,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
         <v>191</v>
       </c>
@@ -1524,7 +1575,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="4" t="s">
         <v>108</v>
       </c>
@@ -1541,7 +1592,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
         <v>115</v>
       </c>
@@ -1558,7 +1609,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="4" t="s">
         <v>116</v>
       </c>
@@ -1575,7 +1626,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
         <v>117</v>
       </c>
@@ -1592,7 +1643,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="4" t="s">
         <v>106</v>
       </c>
@@ -1609,7 +1660,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="4" t="s">
         <v>107</v>
       </c>
@@ -1626,7 +1677,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="4" t="s">
         <v>137</v>
       </c>
@@ -1643,7 +1694,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="28.8">
       <c r="A22" s="4" t="s">
         <v>147</v>
       </c>
@@ -1660,7 +1711,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="28.8">
       <c r="A23" s="4" t="s">
         <v>151</v>
       </c>
@@ -1677,7 +1728,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="4" t="s">
         <v>252</v>
       </c>
@@ -1694,7 +1745,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="4" t="s">
         <v>160</v>
       </c>
@@ -1711,7 +1762,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="4" t="s">
         <v>167</v>
       </c>
@@ -1728,7 +1779,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="4" t="s">
         <v>239</v>
       </c>
@@ -1745,7 +1796,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
         <v>83</v>
       </c>
@@ -1760,7 +1811,7 @@
       </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
         <v>61</v>
       </c>
@@ -1775,7 +1826,7 @@
       </c>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
         <v>77</v>
       </c>
@@ -1790,7 +1841,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
@@ -1805,7 +1856,7 @@
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
         <v>65</v>
       </c>
@@ -1820,7 +1871,7 @@
       </c>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="4" t="s">
         <v>69</v>
       </c>
@@ -1835,7 +1886,7 @@
       </c>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" s="4" t="s">
         <v>73</v>
       </c>
@@ -1850,7 +1901,7 @@
       </c>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" s="4" t="s">
         <v>245</v>
       </c>
@@ -1865,7 +1916,7 @@
       </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" s="7" t="s">
         <v>254</v>
       </c>
@@ -1879,7 +1930,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>172</v>
       </c>
@@ -1893,7 +1944,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>174</v>
       </c>
@@ -1907,7 +1958,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>175</v>
       </c>
@@ -1921,7 +1972,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>179</v>
       </c>
@@ -1935,7 +1986,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>183</v>
       </c>
@@ -1949,7 +2000,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>187</v>
       </c>
@@ -1963,10 +2014,10 @@
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="B44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>25</v>
       </c>
@@ -1980,7 +2031,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -1994,7 +2045,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
         <v>30</v>
       </c>
@@ -2008,7 +2059,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
         <v>32</v>
       </c>
@@ -2022,7 +2073,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>34</v>
       </c>
@@ -2036,7 +2087,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>37</v>
       </c>
@@ -2050,7 +2101,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>40</v>
       </c>
@@ -2064,7 +2115,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>171</v>
       </c>
@@ -2078,7 +2129,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>43</v>
       </c>
@@ -2092,7 +2143,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54" s="12" t="s">
         <v>46</v>
       </c>
@@ -2106,7 +2157,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" s="8" customFormat="1">
       <c r="A56" s="8" t="s">
         <v>195</v>
       </c>
@@ -2120,7 +2171,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>198</v>
       </c>
@@ -2134,7 +2185,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" s="10" customFormat="1">
       <c r="A58" s="10" t="s">
         <v>226</v>
       </c>
@@ -2148,7 +2199,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" s="8" customFormat="1">
       <c r="A59" s="8" t="s">
         <v>220</v>
       </c>
@@ -2162,7 +2213,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" s="8" customFormat="1">
       <c r="A60" s="8" t="s">
         <v>210</v>
       </c>
@@ -2176,7 +2227,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>214</v>
       </c>
@@ -2190,7 +2241,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
         <v>215</v>
       </c>
@@ -2204,7 +2255,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63" s="8" t="s">
         <v>224</v>
       </c>
@@ -2218,7 +2269,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64" s="8" t="s">
         <v>211</v>
       </c>
@@ -2232,7 +2283,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65" s="8" t="s">
         <v>218</v>
       </c>
@@ -2246,7 +2297,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>260</v>
       </c>
@@ -2260,7 +2311,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
         <v>263</v>
       </c>
@@ -2271,7 +2322,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
         <v>265</v>
       </c>
@@ -2282,7 +2333,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
         <v>268</v>
       </c>
@@ -2293,7 +2344,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
         <v>271</v>
       </c>
@@ -2304,7 +2355,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
         <v>274</v>
       </c>
@@ -2315,7 +2366,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4">
       <c r="A74" s="1" t="s">
         <v>277</v>
       </c>
@@ -2326,7 +2377,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4">
       <c r="A75" s="1" t="s">
         <v>280</v>
       </c>
@@ -2335,6 +2386,76 @@
       </c>
       <c r="D75" s="1" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>291</v>
+      </c>
+      <c r="B77" t="s">
+        <v>289</v>
+      </c>
+      <c r="C77" t="s">
+        <v>283</v>
+      </c>
+      <c r="D77" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>